<commit_message>
Ran statistics for Top ZIP Codes - large dataset
</commit_message>
<xml_diff>
--- a/City Comparison NY - SEA - STL.xlsx
+++ b/City Comparison NY - SEA - STL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dutch\Documents\WashU Data Bootcamp\07-Project-1\Project_1_Group_5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82D8602-60F4-4CFC-9FA1-8B8DA2A03032}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF93ECB-1824-432A-B7E9-C459D8899223}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1E1F60BD-E0F7-4694-B899-708778DDB9A6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Results per city</t>
   </si>
@@ -69,17 +69,23 @@
     <t># Businesses</t>
   </si>
   <si>
-    <t># Reviews</t>
-  </si>
-  <si>
     <t>JSON flat files</t>
+  </si>
+  <si>
+    <t>Top 100 zip</t>
+  </si>
+  <si>
+    <t># Reviews*</t>
+  </si>
+  <si>
+    <t>*with male/female gender association</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +101,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -252,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -264,6 +277,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -273,15 +295,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -596,15 +610,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C926860-2BBD-4AC2-85F5-6AEEEF793399}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
@@ -622,48 +636,48 @@
     <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10" t="s">
+      <c r="E2" s="13"/>
+      <c r="F2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10" t="s">
+      <c r="G2" s="13"/>
+      <c r="H2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="11"/>
+      <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="13" t="s">
+      <c r="C3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -676,92 +690,126 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2">
-        <v>378</v>
+        <v>1669</v>
       </c>
       <c r="C5" s="2">
-        <f>D5+E5</f>
-        <v>938</v>
+        <v>3973</v>
       </c>
       <c r="D5" s="4">
-        <v>579</v>
+        <v>2567</v>
       </c>
       <c r="E5" s="5">
-        <v>359</v>
+        <v>1711</v>
       </c>
       <c r="F5" s="4">
-        <v>61.7</v>
+        <v>60</v>
       </c>
       <c r="G5" s="5">
-        <v>38.299999999999997</v>
+        <v>40</v>
       </c>
       <c r="H5" s="2">
-        <v>0.54361609</v>
+        <v>4.4914580000000003E-2</v>
       </c>
       <c r="I5" s="2">
-        <v>0.99149595999999995</v>
+        <v>3.3973719999999999E-2</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B6" s="2">
-        <v>1269</v>
+        <v>378</v>
       </c>
       <c r="C6" s="2">
         <f>D6+E6</f>
-        <v>2995</v>
+        <v>938</v>
       </c>
       <c r="D6" s="4">
-        <v>1853</v>
+        <v>579</v>
       </c>
       <c r="E6" s="5">
-        <v>1142</v>
+        <v>359</v>
       </c>
       <c r="F6" s="4">
-        <v>61.9</v>
+        <v>61.7</v>
       </c>
       <c r="G6" s="5">
-        <v>38.1</v>
+        <v>38.299999999999997</v>
       </c>
       <c r="H6" s="2">
-        <v>0.17377376</v>
+        <v>0.54361609</v>
       </c>
       <c r="I6" s="2">
-        <v>0.16328698</v>
+        <v>0.99149595999999995</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1269</v>
+      </c>
+      <c r="C7" s="2">
+        <f>D7+E7</f>
+        <v>2995</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1853</v>
+      </c>
+      <c r="E7" s="5">
+        <v>1142</v>
+      </c>
+      <c r="F7" s="4">
+        <v>61.9</v>
+      </c>
+      <c r="G7" s="5">
+        <v>38.1</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.17377376</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.16328698</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B8" s="3">
         <v>477</v>
       </c>
-      <c r="C7" s="3">
-        <f>D7+E7</f>
+      <c r="C8" s="3">
+        <f>D8+E8</f>
         <v>1211</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D8" s="6">
         <v>646</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E8" s="7">
         <v>565</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F8" s="6">
         <v>53.3</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G8" s="7">
         <v>46.7</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H8" s="3">
         <v>0.92839578</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I8" s="3">
         <v>0.26738780000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C9" s="15" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>